<commit_message>
Add global  exception handler
</commit_message>
<xml_diff>
--- a/Expense.xlsx
+++ b/Expense.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Expense No.</t>
   </si>
@@ -35,19 +35,34 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Team</t>
+    <t>Payment By</t>
+  </si>
+  <si>
+    <t>#00-8</t>
   </si>
   <si>
     <t>Anuj Pal</t>
   </si>
   <si>
+    <t>My first expense</t>
+  </si>
+  <si>
     <t>Travel Expense</t>
   </si>
   <si>
-    <t>Delhi</t>
+    <t>Attached</t>
   </si>
   <si>
     <t>Hard Cash</t>
+  </si>
+  <si>
+    <t>#00-9</t>
+  </si>
+  <si>
+    <t>#00-10</t>
+  </si>
+  <si>
+    <t>fdgds</t>
   </si>
   <si>
     <t>Food Expense</t>
@@ -114,11 +129,11 @@
     <col min="1" max="1" width="11.87109375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="18.26171875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.69921875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.0625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.0546875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="15.671875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.390625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.7890625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="8.23828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="10.34375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.47265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -148,81 +163,81 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>8.0</v>
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" t="n">
         <v>43468.00208333333</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="n">
         <v>2250.0</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>9.0</v>
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3" t="n">
         <v>43489.001388888886</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="n">
         <v>12250.0</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>10.0</v>
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="B4" t="n">
         <v>43489.001388888886</v>
       </c>
-      <c r="C4" t="n">
-        <v>4355.0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
-        <v>10</v>
+      <c r="G4" t="n">
+        <v>4355.0</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
monitor screen and UI improved
</commit_message>
<xml_diff>
--- a/Expense.xlsx
+++ b/Expense.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Expense No.</t>
   </si>
@@ -38,7 +38,7 @@
     <t>Payment By</t>
   </si>
   <si>
-    <t>#00-8</t>
+    <t>#00-9</t>
   </si>
   <si>
     <t>Anuj Pal</t>
@@ -56,9 +56,6 @@
     <t>Hard Cash</t>
   </si>
   <si>
-    <t>#00-9</t>
-  </si>
-  <si>
     <t>#00-10</t>
   </si>
   <si>
@@ -69,6 +66,36 @@
   </si>
   <si>
     <t>Debit Card</t>
+  </si>
+  <si>
+    <t>#00-11</t>
+  </si>
+  <si>
+    <t>tyw</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>#00-12</t>
+  </si>
+  <si>
+    <t>this is test</t>
+  </si>
+  <si>
+    <t>#00-13</t>
+  </si>
+  <si>
+    <t>sdfghj</t>
+  </si>
+  <si>
+    <t>#00-7</t>
+  </si>
+  <si>
+    <t>Pradip Kumar</t>
+  </si>
+  <si>
+    <t>pradip</t>
   </si>
 </sst>
 </file>
@@ -128,7 +155,7 @@
   <cols>
     <col min="1" max="1" width="11.87109375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="18.26171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.69921875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="15.671875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="14.390625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="10.7890625" customWidth="true" bestFit="true"/>
@@ -167,7 +194,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>43468.00208333333</v>
+        <v>43489.001388888886</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -182,7 +209,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="n">
-        <v>2250.0</v>
+        <v>12250.0</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -199,45 +226,123 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="n">
-        <v>12250.0</v>
+        <v>4355.0</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" t="n">
-        <v>43489.001388888886</v>
+        <v>43490.001388888886</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4" t="n">
-        <v>4355.0</v>
+        <v>5464.0</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="n">
+        <v>43491.001388888886</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="n">
+        <v>567.0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="n">
+        <v>43471.00208333333</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5678.0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>43491.001388888886</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="n">
+        <v>987.0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
home page upgreaded with notification
</commit_message>
<xml_diff>
--- a/Expense.xlsx
+++ b/Expense.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Expense No.</t>
   </si>
   <si>
-    <t>SubmittedDate</t>
+    <t>ApprovedDate</t>
   </si>
   <si>
     <t>Expense Date</t>
@@ -41,48 +41,33 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>#00-10</t>
-  </si>
-  <si>
-    <t>fdgds</t>
+    <t>#00-12</t>
+  </si>
+  <si>
+    <t>this is test</t>
   </si>
   <si>
     <t>Anuj Pal</t>
   </si>
   <si>
+    <t>Travel Expense</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>Attached</t>
+  </si>
+  <si>
+    <t>#00-16</t>
+  </si>
+  <si>
+    <t>effective</t>
+  </si>
+  <si>
     <t>Food Expense</t>
   </si>
   <si>
-    <t>Debit Card</t>
-  </si>
-  <si>
-    <t>Attached</t>
-  </si>
-  <si>
-    <t>#00-11</t>
-  </si>
-  <si>
-    <t>tyw</t>
-  </si>
-  <si>
-    <t>Credit Card</t>
-  </si>
-  <si>
-    <t>#00-12</t>
-  </si>
-  <si>
-    <t>this is test</t>
-  </si>
-  <si>
-    <t>Travel Expense</t>
-  </si>
-  <si>
-    <t>#00-16</t>
-  </si>
-  <si>
-    <t>effective</t>
-  </si>
-  <si>
     <t>Not Attached</t>
   </si>
   <si>
@@ -90,6 +75,12 @@
   </si>
   <si>
     <t>effective two</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -192,10 +183,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>43541.61378472222</v>
+        <v>43541.615219907406</v>
       </c>
       <c r="C2" t="n">
-        <v>43489.001388888886</v>
+        <v>43491.001388888886</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -213,7 +204,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="n">
-        <v>4355.0</v>
+        <v>567.0</v>
       </c>
     </row>
     <row r="3">
@@ -221,10 +212,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>43541.61363425926</v>
+        <v>43541.63195601852</v>
       </c>
       <c r="C3" t="n">
-        <v>43490.001388888886</v>
+        <v>43493.001388888886</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -233,103 +224,74 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I3" t="n">
-        <v>5464.0</v>
+        <v>6576.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="n">
-        <v>43541.61368055556</v>
+        <v>43541.61491898148</v>
       </c>
       <c r="C4" t="n">
-        <v>43491.001388888886</v>
+        <v>43472.00208333333</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
       <c r="I4" t="n">
-        <v>567.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="n">
-        <v>43541.61371527778</v>
-      </c>
-      <c r="C5" t="n">
-        <v>43493.001388888886</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="n">
         <v>6576.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="n">
-        <v>43541.61375</v>
-      </c>
-      <c r="C6" t="n">
-        <v>43472.00208333333</v>
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I6" t="n">
-        <v>6576.0</v>
+        <v>13719.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>